<commit_message>
Fixed some categorization issue
Now using the categories from the given excel
fixed plots
</commit_message>
<xml_diff>
--- a/cleaned_data.xlsx
+++ b/cleaned_data.xlsx
@@ -3351,7 +3351,7 @@
         </is>
       </c>
       <c r="AC27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD27" t="b">
         <v>0</v>
@@ -7187,7 +7187,7 @@
         </is>
       </c>
       <c r="AC63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD63" t="b">
         <v>0</v>
@@ -8991,7 +8991,7 @@
         </is>
       </c>
       <c r="AC80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD80" t="b">
         <v>0</v>
@@ -9831,7 +9831,7 @@
         </is>
       </c>
       <c r="AC88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD88" t="b">
         <v>0</v>
@@ -12807,7 +12807,7 @@
         </is>
       </c>
       <c r="AC116" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD116" t="b">
         <v>0</v>
@@ -13451,7 +13451,7 @@
         </is>
       </c>
       <c r="AC122" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD122" t="b">
         <v>0</v>
@@ -14095,7 +14095,7 @@
         </is>
       </c>
       <c r="AC128" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD128" t="b">
         <v>0</v>

</xml_diff>